<commit_message>
Load life insurance company names only
</commit_message>
<xml_diff>
--- a/assets/保险公司简称.xlsx
+++ b/assets/保险公司简称.xlsx
@@ -1,25 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RH\Desktop\毕业论文\数据\保险科技语料\testPreprocess\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RH\insurtech_tf\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645B857A-53D7-420A-BCF4-92CAEFBD7E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1711D2A0-899F-4591-AFAF-4D8AC58A9466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="财险公司" sheetId="1" r:id="rId1"/>
     <sheet name="寿险公司" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -734,9 +743,6 @@
     <t>泰康人寿保险有限责任公司</t>
   </si>
   <si>
-    <t>中华联合人寿</t>
-  </si>
-  <si>
     <t>信美人寿相互保险社</t>
   </si>
   <si>
@@ -1646,6 +1652,10 @@
   </si>
   <si>
     <t>亚太财险 亚太财保 亚太财产保险公司</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中华人寿</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2015,22 +2025,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="37.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.375" customWidth="1"/>
+    <col min="1" max="1" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" t="s">
         <v>293</v>
-      </c>
-      <c r="B1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2038,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2046,7 +2056,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2054,10 +2064,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2065,7 +2075,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2073,10 +2083,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2084,7 +2094,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2092,15 +2102,15 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2108,7 +2118,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2116,10 +2126,10 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2127,7 +2137,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2135,7 +2145,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2143,7 +2153,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2151,7 +2161,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2159,7 +2169,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2167,10 +2177,10 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2178,10 +2188,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2189,10 +2199,10 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2200,7 +2210,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2208,7 +2218,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2216,7 +2226,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2224,7 +2234,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2232,7 +2242,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2240,7 +2250,7 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2248,7 +2258,7 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2256,7 +2266,7 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2264,7 +2274,7 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2272,7 +2282,7 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2280,7 +2290,7 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2288,7 +2298,7 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2296,7 +2306,7 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2304,10 +2314,10 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2315,7 +2325,7 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2323,10 +2333,10 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2334,7 +2344,7 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2342,7 +2352,7 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2350,7 +2360,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2358,15 +2368,15 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B40" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2374,15 +2384,15 @@
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B42" t="s">
         <v>365</v>
-      </c>
-      <c r="B42" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2390,10 +2400,10 @@
         <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2401,10 +2411,10 @@
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2412,10 +2422,10 @@
         <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2423,7 +2433,7 @@
         <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2431,7 +2441,7 @@
         <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2439,7 +2449,7 @@
         <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2447,18 +2457,18 @@
         <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B50" t="s">
         <v>362</v>
-      </c>
-      <c r="B50" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2466,7 +2476,7 @@
         <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2474,7 +2484,7 @@
         <v>46</v>
       </c>
       <c r="B52" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2482,7 +2492,7 @@
         <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2490,7 +2500,7 @@
         <v>48</v>
       </c>
       <c r="B54" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2498,7 +2508,7 @@
         <v>49</v>
       </c>
       <c r="B55" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2506,7 +2516,7 @@
         <v>50</v>
       </c>
       <c r="B56" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2514,10 +2524,10 @@
         <v>51</v>
       </c>
       <c r="B57" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2525,7 +2535,7 @@
         <v>52</v>
       </c>
       <c r="B58" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2533,7 +2543,7 @@
         <v>53</v>
       </c>
       <c r="B59" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2541,7 +2551,7 @@
         <v>54</v>
       </c>
       <c r="B60" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2549,10 +2559,10 @@
         <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2560,7 +2570,7 @@
         <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2568,7 +2578,7 @@
         <v>57</v>
       </c>
       <c r="B63" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2576,7 +2586,7 @@
         <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2584,7 +2594,7 @@
         <v>59</v>
       </c>
       <c r="B65" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2592,7 +2602,7 @@
         <v>60</v>
       </c>
       <c r="B66" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2600,7 +2610,7 @@
         <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2608,7 +2618,7 @@
         <v>62</v>
       </c>
       <c r="B68" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2616,7 +2626,7 @@
         <v>63</v>
       </c>
       <c r="B69" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2624,7 +2634,7 @@
         <v>64</v>
       </c>
       <c r="B70" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2632,7 +2642,7 @@
         <v>65</v>
       </c>
       <c r="B71" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2640,7 +2650,7 @@
         <v>66</v>
       </c>
       <c r="B72" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2648,7 +2658,7 @@
         <v>67</v>
       </c>
       <c r="B73" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2656,7 +2666,7 @@
         <v>68</v>
       </c>
       <c r="B74" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2664,10 +2674,10 @@
         <v>69</v>
       </c>
       <c r="B75" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2675,7 +2685,7 @@
         <v>70</v>
       </c>
       <c r="B76" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2683,7 +2693,7 @@
         <v>71</v>
       </c>
       <c r="B77" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2691,7 +2701,7 @@
         <v>72</v>
       </c>
       <c r="B78" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2699,7 +2709,7 @@
         <v>73</v>
       </c>
       <c r="B79" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2707,7 +2717,7 @@
         <v>74</v>
       </c>
       <c r="B80" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2715,7 +2725,7 @@
         <v>75</v>
       </c>
       <c r="B81" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2723,7 +2733,7 @@
         <v>76</v>
       </c>
       <c r="B82" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2731,7 +2741,7 @@
         <v>77</v>
       </c>
       <c r="B83" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -2739,7 +2749,7 @@
         <v>78</v>
       </c>
       <c r="B84" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2747,7 +2757,7 @@
         <v>79</v>
       </c>
       <c r="B85" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -2755,7 +2765,7 @@
         <v>80</v>
       </c>
       <c r="B86" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -2763,7 +2773,7 @@
         <v>81</v>
       </c>
       <c r="B87" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2771,7 +2781,7 @@
         <v>82</v>
       </c>
       <c r="B88" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -2785,26 +2795,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D9AA52-6ECE-46A5-A9FB-86A8EEFE6330}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.4140625" customWidth="1"/>
+    <col min="3" max="3" width="49.83203125" customWidth="1"/>
+    <col min="5" max="5" width="58.9140625" customWidth="1"/>
+    <col min="6" max="6" width="30.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B1" t="s">
         <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>387</v>
+        <v>386</v>
+      </c>
+      <c r="D1" t="str">
+        <f>B1&amp;" "&amp;C1</f>
+        <v>中国人寿 中国人寿 中国人寿保险</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>83</v>
@@ -2812,13 +2828,17 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" t="s">
         <v>388</v>
       </c>
-      <c r="B2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C2" t="s">
-        <v>389</v>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D65" si="0">B2&amp;" "&amp;C2</f>
+        <v>中国平安 中国平安 中国平安人寿 平安人寿 中国平安人寿保险 中国平安寿险</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>84</v>
@@ -2829,10 +2849,14 @@
         <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C3" t="s">
-        <v>392</v>
+        <v>391</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>太保寿险 中国太平洋人寿 中国太平洋人寿保险 中国太平洋寿险 太平洋人寿 太平洋人寿保险 太平洋寿险</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>86</v>
@@ -2846,7 +2870,11 @@
         <v>183</v>
       </c>
       <c r="C4" t="s">
-        <v>390</v>
+        <v>389</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>新华人寿 新华人寿 新华人寿保险 新华寿险 新华</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>88</v>
@@ -2854,13 +2882,17 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B5" t="s">
         <v>177</v>
       </c>
       <c r="C5" t="s">
-        <v>391</v>
+        <v>390</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>太平人寿 太平人寿 太平人寿保险 太平寿险 太平</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>89</v>
@@ -2868,13 +2900,17 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B6" t="s">
         <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>393</v>
+        <v>392</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>人保寿险 中国人民人寿 中国人民人寿保险 中国人民寿险</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>90</v>
@@ -2885,10 +2921,14 @@
         <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C7" t="s">
-        <v>394</v>
+        <v>393</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>富德生命 富德生命人寿 富德生命人寿保险 富德寿险 富德生命 富德人寿</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>92</v>
@@ -2902,7 +2942,11 @@
         <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>395</v>
+        <v>394</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>人保健康 中国人民健康保险 中国人保健康</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>94</v>
@@ -2913,10 +2957,14 @@
         <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C9" t="s">
-        <v>396</v>
+        <v>395</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>中国人寿养老 中国人寿养老 中国人寿养老保险</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>96</v>
@@ -2930,7 +2978,11 @@
         <v>173</v>
       </c>
       <c r="C10" t="s">
-        <v>397</v>
+        <v>396</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>民生人寿 民生人寿 民生人寿保险 民生寿险</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>98</v>
@@ -2944,7 +2996,11 @@
         <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>404</v>
+        <v>403</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>阳光人寿 阳光人寿 阳光人寿保险 阳光寿险</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>100</v>
@@ -2958,7 +3014,11 @@
         <v>126</v>
       </c>
       <c r="C12" t="s">
-        <v>405</v>
+        <v>404</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>合众人寿 合众人寿 合众人寿保险 合众寿险</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>102</v>
@@ -2972,7 +3032,11 @@
         <v>233</v>
       </c>
       <c r="C13" t="s">
-        <v>406</v>
+        <v>405</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>百年人寿 百年人寿 百年人寿保险 百年寿险</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>104</v>
@@ -2986,7 +3050,11 @@
         <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>407</v>
+        <v>406</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>中邮人寿 中邮人寿 中邮人寿保险 中邮寿险</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>106</v>
@@ -3000,7 +3068,11 @@
         <v>187</v>
       </c>
       <c r="C15" t="s">
-        <v>398</v>
+        <v>397</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>光大永明 光大永明人寿 光大永明人寿保险 光大永明寿险 光大永明</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>108</v>
@@ -3014,7 +3086,11 @@
         <v>195</v>
       </c>
       <c r="C16" t="s">
-        <v>399</v>
+        <v>398</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>中意人寿 中意人寿 中意人寿保险 中意寿险 中意</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>110</v>
@@ -3025,10 +3101,14 @@
         <v>111</v>
       </c>
       <c r="B17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C17" t="s">
-        <v>400</v>
+        <v>399</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>中美联泰 中美联泰大都会人寿 中美联泰大都会人寿保险 中美联泰大都会寿险 中美联泰大都会</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>112</v>
@@ -3042,7 +3122,11 @@
         <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>401</v>
+        <v>400</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>友邦人寿 友邦人寿 友邦人寿保险 友邦寿险 友邦</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>114</v>
@@ -3056,7 +3140,11 @@
         <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>402</v>
+        <v>401</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>太平养老 太平养老 太平养老保险 太平养老险 太平养老</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>116</v>
@@ -3070,7 +3158,11 @@
         <v>165</v>
       </c>
       <c r="C20" t="s">
-        <v>403</v>
+        <v>402</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>平安养老 平安养老 平安养老保险 平安养老险 平安养老</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>118</v>
@@ -3084,7 +3176,11 @@
         <v>209</v>
       </c>
       <c r="C21" t="s">
-        <v>416</v>
+        <v>415</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>平安健康 平安健康保险 平安健康险</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>120</v>
@@ -3098,7 +3194,11 @@
         <v>139</v>
       </c>
       <c r="C22" t="s">
-        <v>408</v>
+        <v>407</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>天安人寿 天安人寿 天安人寿保险 天安寿险 天安</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>122</v>
@@ -3109,10 +3209,14 @@
         <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C23" t="s">
-        <v>409</v>
+        <v>408</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>大家人寿 大家人寿 大家人寿保险 大家寿险 大家</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>124</v>
@@ -3123,10 +3227,14 @@
         <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C24" t="s">
-        <v>410</v>
+        <v>409</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>英大泰和 英大泰和人寿 英大泰和人寿保险 英大泰和寿险 英大泰和</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>126</v>
@@ -3140,7 +3248,11 @@
         <v>181</v>
       </c>
       <c r="C25" t="s">
-        <v>417</v>
+        <v>416</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>长城人寿 长城人寿 长城人寿保险 长城寿险</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>128</v>
@@ -3154,7 +3266,11 @@
         <v>217</v>
       </c>
       <c r="C26" t="s">
-        <v>411</v>
+        <v>410</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>农银人寿 农银人寿 农银人寿保险 农银寿险 农银</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>130</v>
@@ -3165,10 +3281,14 @@
         <v>131</v>
       </c>
       <c r="B27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C27" t="s">
-        <v>412</v>
+        <v>411</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>君康人寿 君康人寿 君康人寿保险 君康寿险 君康</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>132</v>
@@ -3182,7 +3302,11 @@
         <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>413</v>
+        <v>412</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>华夏人寿 华夏人寿 华夏人寿保险 华夏寿险 华夏</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>134</v>
@@ -3196,7 +3320,11 @@
         <v>185</v>
       </c>
       <c r="C29" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>信泰人寿 信泰人寿 信泰人寿保险 信泰寿险 信泰</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>136</v>
@@ -3210,7 +3338,11 @@
         <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>415</v>
+        <v>414</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>国华人寿 国华人寿 国华人寿保险 国华寿险 国华</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>138</v>
@@ -3218,13 +3350,17 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B31" t="s">
         <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>427</v>
+        <v>426</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">幸福人寿 幸福人寿 幸福人寿保险 幸福寿险 </v>
       </c>
       <c r="F31" s="2" t="s">
         <v>139</v>
@@ -3235,10 +3371,14 @@
         <v>140</v>
       </c>
       <c r="B32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C32" t="s">
-        <v>418</v>
+        <v>417</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>中融人寿 中融人寿 中融人寿保险 中融寿险 中融</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>141</v>
@@ -3252,7 +3392,11 @@
         <v>128</v>
       </c>
       <c r="C33" t="s">
-        <v>419</v>
+        <v>418</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>建信人寿 建信人寿 建信人寿保险 建信寿险 建信</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>143</v>
@@ -3266,7 +3410,11 @@
         <v>86</v>
       </c>
       <c r="C34" t="s">
-        <v>420</v>
+        <v>419</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>利安人寿 利安人寿 利安人寿保险 利安寿险 利安</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>145</v>
@@ -3280,7 +3428,11 @@
         <v>116</v>
       </c>
       <c r="C35" t="s">
-        <v>421</v>
+        <v>420</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>汇丰人寿 汇丰人寿 汇丰人寿保险 汇丰寿险 汇丰</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>147</v>
@@ -3294,7 +3446,11 @@
         <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>422</v>
+        <v>421</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>中宏人寿 中宏人寿 中宏人寿保险 中宏寿险 中宏</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>149</v>
@@ -3305,10 +3461,14 @@
         <v>150</v>
       </c>
       <c r="B37" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C37" t="s">
-        <v>423</v>
+        <v>422</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>安联人寿 安联人寿 安联人寿保险 安联寿险 安联</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>151</v>
@@ -3322,7 +3482,11 @@
         <v>193</v>
       </c>
       <c r="C38" t="s">
-        <v>424</v>
+        <v>423</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>工银安盛 工银安盛人寿 工银安盛人寿保险 工银安盛寿险 工银安盛</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>153</v>
@@ -3333,10 +3497,14 @@
         <v>154</v>
       </c>
       <c r="B39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C39" t="s">
-        <v>425</v>
+        <v>424</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>中信保诚 中信保诚人寿 中信保诚人寿保险 中信保诚寿险 中信保诚</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>155</v>
@@ -3350,7 +3518,11 @@
         <v>149</v>
       </c>
       <c r="C40" t="s">
-        <v>426</v>
+        <v>425</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>交银人寿 交银人寿 交银人寿保险 交银寿险 交银</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>157</v>
@@ -3364,7 +3536,11 @@
         <v>197</v>
       </c>
       <c r="C41" t="s">
-        <v>428</v>
+        <v>427</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>中荷人寿 中荷人寿 中荷人寿保险 中荷寿险 中荷</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>159</v>
@@ -3375,10 +3551,14 @@
         <v>160</v>
       </c>
       <c r="B42" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C42" t="s">
-        <v>429</v>
+        <v>428</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>同方全球 同方全球人寿 同方全球人寿保险 同方全球寿险 同方全球</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>161</v>
@@ -3392,7 +3572,11 @@
         <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>430</v>
+        <v>429</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>中英人寿 中英人寿 中英人寿保险 中英寿险 中英</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>163</v>
@@ -3403,10 +3587,14 @@
         <v>164</v>
       </c>
       <c r="B44" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C44" t="s">
-        <v>431</v>
+        <v>430</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>恒安标准 恒安标准人寿 恒安标准人寿保险 恒安标准寿险 恒安标准</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>165</v>
@@ -3417,10 +3605,14 @@
         <v>166</v>
       </c>
       <c r="B45" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C45" t="s">
-        <v>432</v>
+        <v>431</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>招商信诺 招商信诺人寿 招商信诺人寿保险 招商信诺寿险 招商信诺</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>167</v>
@@ -3431,10 +3623,14 @@
         <v>168</v>
       </c>
       <c r="B46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C46" t="s">
-        <v>433</v>
+        <v>432</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>陆家嘴国泰 陆家嘴国泰人寿 陆家嘴国泰人寿保险 陆家嘴国泰寿险 陆家嘴国泰</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>169</v>
@@ -3448,7 +3644,11 @@
         <v>112</v>
       </c>
       <c r="C47" t="s">
-        <v>434</v>
+        <v>433</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>华泰人寿 华泰人寿 华泰人寿保险 华泰寿险 华泰</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>171</v>
@@ -3459,10 +3659,14 @@
         <v>172</v>
       </c>
       <c r="B48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C48" t="s">
-        <v>435</v>
+        <v>434</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>中银三星 中银三星人寿 中银三星人寿保险 中银三星寿险 中银三星</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>173</v>
@@ -3476,7 +3680,11 @@
         <v>122</v>
       </c>
       <c r="C49" t="s">
-        <v>436</v>
+        <v>435</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>泰康养老 泰康养老 泰康养老保险 泰康养老险</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>175</v>
@@ -3490,7 +3698,11 @@
         <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>437</v>
+        <v>436</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>长江养老 长江养老 长江养老保险 长江养老险</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>177</v>
@@ -3501,10 +3713,14 @@
         <v>178</v>
       </c>
       <c r="B51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C51" t="s">
-        <v>444</v>
+        <v>443</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>和谐健康 和谐健康 和谐健康保险 和谐健康险</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>179</v>
@@ -3515,10 +3731,14 @@
         <v>180</v>
       </c>
       <c r="B52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C52" t="s">
-        <v>445</v>
+        <v>444</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>昆仑健康 昆仑健康 昆仑健康保险 昆仑健康险</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>181</v>
@@ -3532,7 +3752,11 @@
         <v>201</v>
       </c>
       <c r="C53" t="s">
-        <v>446</v>
+        <v>445</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>瑞泰人寿 瑞泰人寿 瑞泰人寿保险 瑞泰寿险 瑞泰</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>183</v>
@@ -3543,10 +3767,14 @@
         <v>184</v>
       </c>
       <c r="B54" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C54" t="s">
-        <v>438</v>
+        <v>437</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>北大方正 北大方正人寿 北大方正人寿保险 北大方正寿险 北大方正</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>185</v>
@@ -3560,7 +3788,11 @@
         <v>161</v>
       </c>
       <c r="C55" t="s">
-        <v>439</v>
+        <v>438</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>君龙人寿 君龙人寿 君龙人寿保险 君龙寿险 君龙</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>187</v>
@@ -3574,7 +3806,11 @@
         <v>215</v>
       </c>
       <c r="C56" t="s">
-        <v>440</v>
+        <v>439</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>华汇人寿 华汇人寿 华汇人寿保险 华汇寿险 华汇</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>189</v>
@@ -3588,7 +3824,11 @@
         <v>134</v>
       </c>
       <c r="C57" t="s">
-        <v>441</v>
+        <v>440</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>前海人寿 前海人寿 前海人寿保险 前海寿险 前海</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>191</v>
@@ -3602,7 +3842,11 @@
         <v>189</v>
       </c>
       <c r="C58" t="s">
-        <v>442</v>
+        <v>441</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>东吴人寿 东吴人寿 东吴人寿保险 东吴寿险 东吴</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>193</v>
@@ -3616,7 +3860,11 @@
         <v>171</v>
       </c>
       <c r="C59" t="s">
-        <v>443</v>
+        <v>442</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>弘康人寿 弘康人寿 弘康人寿保险 弘康寿险 弘康</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>195</v>
@@ -3627,10 +3875,14 @@
         <v>196</v>
       </c>
       <c r="B60" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C60" t="s">
-        <v>447</v>
+        <v>446</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>财信人寿 财信吉祥人寿 财信吉祥人寿保险 财信吉祥寿险 财信吉祥</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>197</v>
@@ -3644,7 +3896,11 @@
         <v>207</v>
       </c>
       <c r="C61" t="s">
-        <v>453</v>
+        <v>452</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>复星保德信 复星保德信 复星保德信人寿 复星保德信寿险</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>199</v>
@@ -3655,10 +3911,14 @@
         <v>200</v>
       </c>
       <c r="B62" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C62" t="s">
-        <v>448</v>
+        <v>447</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>中韩人寿 中韩人寿 中韩人寿保险 中韩寿险 中韩</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>201</v>
@@ -3672,7 +3932,11 @@
         <v>136</v>
       </c>
       <c r="C63" t="s">
-        <v>449</v>
+        <v>448</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>珠江人寿 珠江人寿 珠江人寿保险 珠江寿险 珠江</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>203</v>
@@ -3683,10 +3947,14 @@
         <v>204</v>
       </c>
       <c r="B64" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C64" t="s">
-        <v>450</v>
+        <v>449</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>德华安顾 德华安顾 德华安顾人寿 德华寿险 德华安顾</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>205</v>
@@ -3700,7 +3968,11 @@
         <v>110</v>
       </c>
       <c r="C65" t="s">
-        <v>454</v>
+        <v>453</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>长生人寿 长生人寿 长生人寿保险 长生寿险</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>207</v>
@@ -3711,10 +3983,14 @@
         <v>208</v>
       </c>
       <c r="B66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C66" t="s">
-        <v>455</v>
+        <v>454</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" ref="D66:D92" si="1">B66&amp;" "&amp;C66</f>
+        <v>小康人寿 小康人寿 小康人寿保险 小康寿险</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>209</v>
@@ -3728,7 +4004,11 @@
         <v>145</v>
       </c>
       <c r="C67" t="s">
-        <v>456</v>
+        <v>455</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="1"/>
+        <v>上海人寿 上海人寿 上海人寿保险 上海寿险</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>211</v>
@@ -3742,7 +4022,11 @@
         <v>231</v>
       </c>
       <c r="C68" t="s">
-        <v>451</v>
+        <v>450</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="1"/>
+        <v>国联人寿 国联人寿 国联人寿保险 国联寿险 国联</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>213</v>
@@ -3756,7 +4040,11 @@
         <v>225</v>
       </c>
       <c r="C69" t="s">
-        <v>457</v>
+        <v>456</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="1"/>
+        <v>渤海人寿 渤海人寿 渤海人寿保险 渤海寿险 渤海</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>215</v>
@@ -3767,10 +4055,14 @@
         <v>216</v>
       </c>
       <c r="B70" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C70" t="s">
-        <v>452</v>
+        <v>451</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>中华联合 中华联合 中华联合人寿 中华联合寿险 中华联合</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>217</v>
@@ -3781,10 +4073,14 @@
         <v>218</v>
       </c>
       <c r="B71" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C71" t="s">
-        <v>463</v>
+        <v>462</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>大家养老 大家养老 大家养老保险 大家养老险</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>219</v>
@@ -3795,10 +4091,14 @@
         <v>220</v>
       </c>
       <c r="B72" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C72" t="s">
-        <v>464</v>
+        <v>463</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="1"/>
+        <v>太保健康 太平洋健康 太平洋健康保险 太平洋健康险</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>221</v>
@@ -3809,10 +4109,14 @@
         <v>222</v>
       </c>
       <c r="B73" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C73" t="s">
-        <v>458</v>
+        <v>457</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>恒大人寿 恒大人寿 恒大人寿保险 恒大寿险 恒大</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>223</v>
@@ -3823,10 +4127,14 @@
         <v>224</v>
       </c>
       <c r="B74" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C74" t="s">
-        <v>459</v>
+        <v>458</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>鼎诚人寿 鼎诚人寿 鼎诚人寿保险 鼎诚寿险 鼎诚</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>225</v>
@@ -3837,10 +4145,14 @@
         <v>226</v>
       </c>
       <c r="B75" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C75" t="s">
-        <v>460</v>
+        <v>459</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="1"/>
+        <v>横琴人寿 横琴人寿 横琴人寿保险 横琴寿险 横琴</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>227</v>
@@ -3854,7 +4166,11 @@
         <v>213</v>
       </c>
       <c r="C76" t="s">
-        <v>465</v>
+        <v>464</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="1"/>
+        <v>新华养老 新华养老 新华养老保险 新华养老险</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>229</v>
@@ -3868,7 +4184,11 @@
         <v>100</v>
       </c>
       <c r="C77" t="s">
-        <v>461</v>
+        <v>460</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="1"/>
+        <v>华贵人寿 华贵人寿 华贵人寿保险 华贵寿险 华贵</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>231</v>
@@ -3879,10 +4199,14 @@
         <v>232</v>
       </c>
       <c r="B78" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C78" t="s">
-        <v>466</v>
+        <v>465</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="1"/>
+        <v>复星联合 复星联合健康 复星联合健康保险 复星联合健康险</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>233</v>
@@ -3896,192 +4220,248 @@
         <v>94</v>
       </c>
       <c r="C79" t="s">
-        <v>462</v>
+        <v>461</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="1"/>
+        <v>泰康人寿 泰康人寿 泰康人寿保险 泰康寿险 泰康</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>235</v>
+        <v>494</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B80" t="s">
         <v>191</v>
       </c>
       <c r="C80" t="s">
-        <v>467</v>
+        <v>466</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="1"/>
+        <v>信美人寿 信美人寿 信美 信美相互</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
+        <v>237</v>
+      </c>
+      <c r="B81" t="s">
+        <v>270</v>
+      </c>
+      <c r="C81" t="s">
+        <v>470</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>招商仁和 招商局仁和 招商局仁和人寿 招商局仁和寿险</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="B81" t="s">
-        <v>271</v>
-      </c>
-      <c r="C81" t="s">
-        <v>471</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
+        <v>239</v>
+      </c>
+      <c r="B82" t="s">
+        <v>272</v>
+      </c>
+      <c r="C82" t="s">
+        <v>467</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>和泰人寿 和泰人寿 和泰人寿保险 和泰寿险 和泰</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="B82" t="s">
-        <v>273</v>
-      </c>
-      <c r="C82" t="s">
-        <v>468</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B83" t="s">
         <v>219</v>
       </c>
       <c r="C83" t="s">
-        <v>472</v>
+        <v>471</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>爱心人寿 爱心人寿 爱心人寿保险 爱心寿险</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
+        <v>243</v>
+      </c>
+      <c r="B84" t="s">
+        <v>271</v>
+      </c>
+      <c r="C84" t="s">
+        <v>472</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>中国人民养老 中国人民养老保险 中国人民养老险</v>
+      </c>
+      <c r="F84" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B84" t="s">
-        <v>272</v>
-      </c>
-      <c r="C84" t="s">
-        <v>473</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B85" t="s">
         <v>221</v>
       </c>
       <c r="C85" t="s">
-        <v>475</v>
+        <v>474</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>三峡人寿 三峡人寿 三峡人寿保险 三峡寿险</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B86" t="s">
         <v>223</v>
       </c>
       <c r="C86" t="s">
-        <v>474</v>
+        <v>473</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>北京人寿 北京人寿 北京人寿保险 北京寿险</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
+        <v>249</v>
+      </c>
+      <c r="B87" t="s">
+        <v>260</v>
+      </c>
+      <c r="C87" t="s">
+        <v>468</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>海保人寿 海保人寿 海保人寿保险 海保寿险 海保</v>
+      </c>
+      <c r="F87" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B87" t="s">
-        <v>261</v>
-      </c>
-      <c r="C87" t="s">
-        <v>469</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
+        <v>251</v>
+      </c>
+      <c r="B88" t="s">
+        <v>240</v>
+      </c>
+      <c r="C88" t="s">
+        <v>475</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>瑞华健康 瑞华健康 瑞华健康保险 瑞华健康险</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="B88" t="s">
-        <v>241</v>
-      </c>
-      <c r="C88" t="s">
-        <v>476</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B89" t="s">
         <v>227</v>
       </c>
       <c r="C89" t="s">
-        <v>477</v>
+        <v>476</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="1"/>
+        <v>国宝人寿 国宝人寿 国宝人寿保险 国宝寿险</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B90" t="s">
         <v>229</v>
       </c>
       <c r="C90" t="s">
-        <v>470</v>
+        <v>469</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="1"/>
+        <v>国富人寿 国富人寿 国富人寿保险 国富寿险 国富</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
+        <v>257</v>
+      </c>
+      <c r="B91" t="s">
+        <v>282</v>
+      </c>
+      <c r="C91" t="s">
+        <v>477</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="1"/>
+        <v>恒安标准 恒安标准养老 恒安标准养老保险 恒安标准养老险</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="B91" t="s">
-        <v>283</v>
-      </c>
-      <c r="C91" t="s">
-        <v>478</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B92" t="s">
         <v>211</v>
       </c>
       <c r="C92" t="s">
-        <v>479</v>
+        <v>478</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="1"/>
+        <v>国民养老 国民养老 国民养老保险 国民养老险</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>